<commit_message>
read_data function and sadata data
</commit_message>
<xml_diff>
--- a/replication_summary_allWV_annotation.xlsx
+++ b/replication_summary_allWV_annotation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-18260" yWindow="-5000" windowWidth="18140" windowHeight="23140" tabRatio="500"/>
+    <workbookView xWindow="-580" yWindow="680" windowWidth="18140" windowHeight="23140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="replication_summary_allWV.csv" sheetId="1" r:id="rId1"/>
@@ -757,8 +757,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D49" activeCellId="1" sqref="B49 D49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>